<commit_message>
Updated data at 9:30 PM
</commit_message>
<xml_diff>
--- a/December2020/AGNOOR.xlsx
+++ b/December2020/AGNOOR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="4" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Pawan &amp; Ravi - (660604868)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="19">
   <si>
     <t>pawan and ravi telicom-(660604868)</t>
   </si>
@@ -84,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -113,8 +113,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,8 +138,90 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,92 +235,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,15 +248,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,7 +276,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,31 +306,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,139 +432,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,37 +494,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,9 +520,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,12 +558,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -596,134 +590,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -742,9 +736,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -761,9 +752,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1097,7 +1085,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1108,14 +1096,14 @@
     <col min="5" max="5" width="17.2857142857143" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="16382" width="9.14285714285714" style="1"/>
-    <col min="16383" max="16384" width="9.14285714285714" style="15"/>
+    <col min="16383" max="16384" width="9.14285714285714" style="13"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -1137,26 +1125,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:6">
-      <c r="A3" s="6" t="s">
+    <row r="3" s="2" customFormat="1" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>44167</v>
       </c>
       <c r="B4" s="1">
         <v>2080</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>2000</v>
       </c>
@@ -1165,7 +1148,7 @@
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>44168</v>
       </c>
       <c r="B5" s="1">
@@ -1179,10 +1162,9 @@
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:5">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>44168</v>
       </c>
-      <c r="B6" s="1"/>
       <c r="C6" s="1">
         <v>2000</v>
       </c>
@@ -1194,13 +1176,12 @@
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:5">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>44169</v>
       </c>
       <c r="B7" s="1">
         <v>4160</v>
       </c>
-      <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>6000</v>
       </c>
@@ -1209,13 +1190,12 @@
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:5">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>44169</v>
       </c>
       <c r="B8" s="1">
         <v>1040</v>
       </c>
-      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>7000</v>
       </c>
@@ -1224,13 +1204,12 @@
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:5">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>44170</v>
       </c>
       <c r="B9" s="1">
         <v>1040</v>
       </c>
-      <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>8000</v>
       </c>
@@ -1239,13 +1218,12 @@
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:5">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>44170</v>
       </c>
       <c r="B10" s="1">
         <v>1040</v>
       </c>
-      <c r="C10" s="1"/>
       <c r="D10" s="1">
         <v>9000</v>
       </c>
@@ -1254,13 +1232,12 @@
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:5">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>44171</v>
       </c>
       <c r="B11" s="1">
         <v>3120</v>
       </c>
-      <c r="C11" s="1"/>
       <c r="D11" s="1">
         <v>12000</v>
       </c>
@@ -1268,18 +1245,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1"/>
+    <row r="12" s="1" customFormat="1" spans="1:5">
+      <c r="A12" s="6">
+        <v>44172</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5200</v>
+      </c>
+      <c r="D12" s="1">
+        <v>17000</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="13" s="1" customFormat="1"/>
     <row r="14" s="1" customFormat="1"/>
-    <row r="15" s="15" customFormat="1"/>
-    <row r="16" s="15" customFormat="1"/>
-    <row r="17" s="15" customFormat="1"/>
-    <row r="18" s="15" customFormat="1"/>
-    <row r="19" s="15" customFormat="1"/>
-    <row r="20" s="15" customFormat="1"/>
-    <row r="21" s="15" customFormat="1"/>
-    <row r="22" s="15" customFormat="1"/>
-    <row r="23" s="15" customFormat="1"/>
+    <row r="15" s="13" customFormat="1"/>
+    <row r="16" s="13" customFormat="1"/>
+    <row r="17" s="13" customFormat="1"/>
+    <row r="18" s="13" customFormat="1"/>
+    <row r="19" s="13" customFormat="1"/>
+    <row r="20" s="13" customFormat="1"/>
+    <row r="21" s="13" customFormat="1"/>
+    <row r="22" s="13" customFormat="1"/>
+    <row r="23" s="13" customFormat="1"/>
     <row r="24" s="1" customFormat="1"/>
     <row r="25" s="1" customFormat="1"/>
     <row r="26" s="1" customFormat="1"/>
@@ -1304,10 +1294,10 @@
     <row r="45" customFormat="1"/>
     <row r="46" customFormat="1"/>
     <row r="47" s="1" customFormat="1" spans="1:1">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
     </row>
     <row r="48" s="1" customFormat="1" spans="1:1">
-      <c r="A48" s="7"/>
+      <c r="A48" s="6"/>
     </row>
     <row r="49" s="1" customFormat="1"/>
     <row r="50" customFormat="1"/>
@@ -1315,7 +1305,7 @@
     <row r="52" customFormat="1"/>
     <row r="53" customFormat="1"/>
     <row r="54" s="1" customFormat="1" spans="1:1">
-      <c r="A54" s="7"/>
+      <c r="A54" s="6"/>
     </row>
     <row r="55" s="1" customFormat="1"/>
     <row r="56" s="1" customFormat="1"/>
@@ -1323,12 +1313,12 @@
     <row r="58" customFormat="1"/>
     <row r="59" customFormat="1"/>
     <row r="60" s="1" customFormat="1" spans="1:1">
-      <c r="A60" s="7"/>
+      <c r="A60" s="6"/>
     </row>
     <row r="61" s="1" customFormat="1"/>
     <row r="62" s="1" customFormat="1"/>
     <row r="63" s="1" customFormat="1" spans="1:1">
-      <c r="A63" s="7"/>
+      <c r="A63" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1342,10 +1332,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1360,12 +1350,12 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -1387,20 +1377,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="1" spans="1:6">
-      <c r="A3" s="13" t="s">
+    <row r="3" s="9" customFormat="1" spans="1:4">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13">
+      <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>44167</v>
       </c>
       <c r="B4" s="1">
@@ -1414,7 +1400,7 @@
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>44167</v>
       </c>
       <c r="B5" s="1">
@@ -1428,7 +1414,7 @@
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:5">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>44168</v>
       </c>
       <c r="B6" s="1">
@@ -1442,7 +1428,7 @@
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:5">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>44168</v>
       </c>
       <c r="B7" s="1">
@@ -1456,7 +1442,7 @@
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:5">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>44168</v>
       </c>
       <c r="B8" s="1">
@@ -1470,7 +1456,7 @@
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:5">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>44168</v>
       </c>
       <c r="C9" s="1">
@@ -1484,7 +1470,7 @@
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:5">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>44169</v>
       </c>
       <c r="B10" s="1">
@@ -1498,7 +1484,7 @@
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:5">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>44169</v>
       </c>
       <c r="B11" s="1">
@@ -1512,7 +1498,7 @@
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:5">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>44170</v>
       </c>
       <c r="B12" s="1">
@@ -1526,7 +1512,7 @@
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:5">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>44170</v>
       </c>
       <c r="C13" s="1">
@@ -1540,7 +1526,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>44171</v>
       </c>
       <c r="C14" s="3">
@@ -1554,7 +1540,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>44171</v>
       </c>
       <c r="B15" s="3">
@@ -1564,6 +1550,20 @@
         <v>3000</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B16" s="3">
+        <v>5200</v>
+      </c>
+      <c r="D16" s="3">
+        <v>8000</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1580,13 +1580,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1597,11 +1597,11 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -1623,20 +1623,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="1" spans="1:6">
-      <c r="A3" s="13" t="s">
+    <row r="3" s="9" customFormat="1" spans="1:4">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13">
+      <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>44168</v>
       </c>
       <c r="B4" s="1">
@@ -1650,7 +1646,7 @@
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>44168</v>
       </c>
       <c r="C5" s="1">
@@ -1664,7 +1660,7 @@
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:5">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>44170</v>
       </c>
       <c r="C6" s="1">
@@ -1675,6 +1671,20 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6">
+        <v>44172</v>
+      </c>
+      <c r="B7">
+        <v>2080</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1690,10 +1700,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1707,144 +1717,140 @@
     <col min="7" max="16384" width="9.14285714285714" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" spans="1:2">
-      <c r="A1" s="11" t="s">
+    <row r="1" s="8" customFormat="1" spans="1:2">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" s="9" customFormat="1" spans="1:6">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" s="8" customFormat="1" spans="1:6">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="1" spans="1:6">
-      <c r="A3" s="13" t="s">
+    <row r="3" s="9" customFormat="1" spans="1:4">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13">
+      <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" s="9" customFormat="1" spans="1:5">
-      <c r="A4" s="14">
+    </row>
+    <row r="4" s="8" customFormat="1" spans="1:5">
+      <c r="A4" s="12">
         <v>44167</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>2080</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>2000</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" s="9" customFormat="1" spans="1:5">
-      <c r="A5" s="14">
+    <row r="5" s="8" customFormat="1" spans="1:5">
+      <c r="A5" s="12">
         <v>44168</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>1040</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>3000</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" s="9" customFormat="1" spans="1:5">
-      <c r="A6" s="14">
+    <row r="6" s="8" customFormat="1" spans="1:5">
+      <c r="A6" s="12">
         <v>44168</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>2000</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>1000</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" s="9" customFormat="1" spans="1:5">
-      <c r="A7" s="14">
+    <row r="7" s="8" customFormat="1" spans="1:5">
+      <c r="A7" s="12">
         <v>44169</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>1040</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>2000</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" s="9" customFormat="1" spans="1:5">
-      <c r="A8" s="14">
+    <row r="8" s="8" customFormat="1" spans="1:5">
+      <c r="A8" s="12">
         <v>44169</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>2080</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>4000</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" s="9" customFormat="1" spans="1:5">
-      <c r="A9" s="14">
+    <row r="9" s="8" customFormat="1" spans="1:5">
+      <c r="A9" s="12">
         <v>44170</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>1040</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>5000</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" s="9" customFormat="1" spans="1:5">
-      <c r="A10" s="14">
+    <row r="10" s="8" customFormat="1" spans="1:5">
+      <c r="A10" s="12">
         <v>44170</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>4000</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>1000</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="14">
+      <c r="A11" s="12">
         <v>44171</v>
       </c>
       <c r="B11" s="3">
@@ -1854,6 +1860,20 @@
         <v>4000</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12">
+        <v>44173</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5200</v>
+      </c>
+      <c r="D12" s="3">
+        <v>9000</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1913,20 +1933,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:6">
-      <c r="A3" s="6" t="s">
+    <row r="3" s="2" customFormat="1" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>44168</v>
       </c>
       <c r="B4" s="1">
@@ -1940,7 +1956,7 @@
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>44168</v>
       </c>
       <c r="C5" s="1">
@@ -1954,7 +1970,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>44171</v>
       </c>
       <c r="B6" s="3">
@@ -1982,7 +1998,7 @@
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1997,11 +2013,11 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -2023,20 +2039,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:6">
-      <c r="A3" s="6" t="s">
+    <row r="3" s="2" customFormat="1" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>44171</v>
       </c>
       <c r="B4" s="1">
@@ -2064,8 +2076,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -2106,20 +2118,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:6">
-      <c r="A3" s="6" t="s">
+    <row r="3" s="2" customFormat="1" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>44171</v>
       </c>
       <c r="B4" s="1">
@@ -2133,7 +2141,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>44171</v>
       </c>
       <c r="C5" s="3">

</xml_diff>

<commit_message>
Updated till 10 Dec 8AM
</commit_message>
<xml_diff>
--- a/December2020/AGNOOR.xlsx
+++ b/December2020/AGNOOR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="4" activeTab="6"/>
+    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pawan &amp; Ravi - (660604868)" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="SINGH TELECOM-(661066803)" sheetId="5" r:id="rId5"/>
     <sheet name="PRABHAT TELECOM -(661066820)" sheetId="6" r:id="rId6"/>
     <sheet name="SAJNISH KIRANA-(661644709)" sheetId="8" r:id="rId7"/>
+    <sheet name="S K Mobile" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="20">
   <si>
     <t>pawan and ravi telicom-(660604868)</t>
   </si>
@@ -34,10 +35,10 @@
     <t>Receive Amount</t>
   </si>
   <si>
-    <t>Dues Amount</t>
+    <t>Transaction Type</t>
   </si>
   <si>
-    <t>Transaction Type</t>
+    <t>Dues Amount</t>
   </si>
   <si>
     <t>Remarks</t>
@@ -53,6 +54,9 @@
   </si>
   <si>
     <t>Auto</t>
+  </si>
+  <si>
+    <t>Digital</t>
   </si>
   <si>
     <t>ARVIND AIRTEL EGRECHARGE CENTRE-(661591709)</t>
@@ -76,7 +80,7 @@
     <t>SAJNISH KIRANA-(661644709)</t>
   </si>
   <si>
-    <t>Digital</t>
+    <t>G Pay</t>
   </si>
 </sst>
 </file>
@@ -85,10 +89,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -106,15 +110,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -129,11 +125,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -145,15 +141,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,10 +158,33 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,9 +195,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,7 +211,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,6 +219,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,29 +246,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -276,181 +280,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,35 +500,29 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -559,11 +557,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,15 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -590,130 +594,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -739,8 +743,8 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1085,15 +1089,16 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="4" width="16.8571428571429" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8571428571429" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.8571428571429" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="16382" width="9.14285714285714" style="1"/>
     <col min="16383" max="16384" width="9.14285714285714" style="13"/>
@@ -1125,11 +1130,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:4">
+    <row r="3" s="2" customFormat="1" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1140,11 +1145,11 @@
       <c r="B4" s="1">
         <v>2080</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>2000</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
@@ -1154,11 +1159,11 @@
       <c r="B5" s="1">
         <v>2080</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
         <v>4000</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:5">
@@ -1168,11 +1173,11 @@
       <c r="C6" s="1">
         <v>2000</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
         <v>2000</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:5">
@@ -1182,11 +1187,11 @@
       <c r="B7" s="1">
         <v>4160</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
         <v>6000</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:5">
@@ -1196,11 +1201,11 @@
       <c r="B8" s="1">
         <v>1040</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
         <v>7000</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:5">
@@ -1210,11 +1215,11 @@
       <c r="B9" s="1">
         <v>1040</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
         <v>8000</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:5">
@@ -1224,11 +1229,11 @@
       <c r="B10" s="1">
         <v>1040</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
         <v>9000</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:5">
@@ -1238,11 +1243,11 @@
       <c r="B11" s="1">
         <v>3120</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
         <v>12000</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:5">
@@ -1252,15 +1257,41 @@
       <c r="B12" s="1">
         <v>5200</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
         <v>17000</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1"/>
-    <row r="14" s="1" customFormat="1"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:5">
+      <c r="A13" s="6">
+        <v>44174</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3000</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:5">
+      <c r="A14" s="6">
+        <v>44174</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11000</v>
+      </c>
+    </row>
     <row r="15" s="13" customFormat="1"/>
     <row r="16" s="13" customFormat="1"/>
     <row r="17" s="13" customFormat="1"/>
@@ -1332,26 +1363,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="17" style="3" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.8571428571429" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.14285714285714" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.14285714285714" style="3"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1377,11 +1408,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="9" customFormat="1" spans="1:4">
+    <row r="3" s="9" customFormat="1" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E3" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1392,11 +1423,11 @@
       <c r="B4" s="1">
         <v>1040</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>1000</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
@@ -1406,25 +1437,28 @@
       <c r="B5" s="1">
         <v>520</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
         <v>1500</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:5">
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="6">
         <v>44168</v>
       </c>
       <c r="B6" s="1">
         <v>520</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
         <v>2000</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
+      <c r="H6" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:5">
@@ -1434,11 +1468,11 @@
       <c r="B7" s="1">
         <v>520</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
         <v>2500</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:5">
@@ -1448,11 +1482,11 @@
       <c r="B8" s="1">
         <v>1040</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
         <v>3500</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:5">
@@ -1462,11 +1496,11 @@
       <c r="C9" s="1">
         <v>3000</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1">
         <v>500</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:5">
@@ -1476,11 +1510,11 @@
       <c r="B10" s="1">
         <v>2080</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
         <v>2500</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:5">
@@ -1490,11 +1524,11 @@
       <c r="B11" s="1">
         <v>1040</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
         <v>3500</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:5">
@@ -1504,11 +1538,11 @@
       <c r="B12" s="1">
         <v>1040</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
         <v>4500</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:5">
@@ -1518,11 +1552,11 @@
       <c r="C13" s="1">
         <v>2000</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
         <v>2500</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1532,11 +1566,11 @@
       <c r="C14" s="3">
         <v>1500</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3">
         <v>1000</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1546,11 +1580,11 @@
       <c r="B15" s="3">
         <v>2080</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3">
         <v>3000</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1560,11 +1594,25 @@
       <c r="B16" s="3">
         <v>5200</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
         <v>8000</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>10</v>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="6">
+        <v>44174</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4000</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3">
+        <v>4000</v>
       </c>
     </row>
   </sheetData>
@@ -1580,28 +1628,29 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="16.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
+    <col min="1" max="1" width="17" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.8571428571429" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="9.14285714285714" style="7"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -1623,11 +1672,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="9" customFormat="1" spans="1:4">
+    <row r="3" s="9" customFormat="1" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E3" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1638,11 +1687,11 @@
       <c r="B4" s="1">
         <v>2080</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>2000</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
@@ -1652,11 +1701,11 @@
       <c r="C5" s="1">
         <v>1000</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
         <v>1000</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:5">
@@ -1666,25 +1715,39 @@
       <c r="C6" s="1">
         <v>1000</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
         <v>0</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6">
         <v>44172</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7">
         <v>2080</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7">
         <v>2000</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="6">
+        <v>44174</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1700,10 +1763,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D1" sqref="D$1:D$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1711,15 +1774,15 @@
     <col min="1" max="1" width="32.1428571428571" style="3" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.8571428571429" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.14285714285714" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.14285714285714" style="3"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="1" spans="1:2">
       <c r="A1" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="10"/>
     </row>
@@ -1743,11 +1806,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="9" customFormat="1" spans="1:4">
+    <row r="3" s="9" customFormat="1" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E3" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1758,11 +1821,11 @@
       <c r="B4" s="8">
         <v>2080</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8">
         <v>2000</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" s="8" customFormat="1" spans="1:5">
@@ -1772,11 +1835,11 @@
       <c r="B5" s="8">
         <v>1040</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8">
         <v>3000</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" s="8" customFormat="1" spans="1:5">
@@ -1786,11 +1849,11 @@
       <c r="C6" s="8">
         <v>2000</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8">
         <v>1000</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" s="8" customFormat="1" spans="1:5">
@@ -1800,11 +1863,11 @@
       <c r="B7" s="8">
         <v>1040</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="8">
         <v>2000</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" s="8" customFormat="1" spans="1:5">
@@ -1814,11 +1877,11 @@
       <c r="B8" s="8">
         <v>2080</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8">
         <v>4000</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" s="8" customFormat="1" spans="1:5">
@@ -1828,11 +1891,11 @@
       <c r="B9" s="8">
         <v>1040</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="8">
         <v>5000</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" s="8" customFormat="1" spans="1:5">
@@ -1842,11 +1905,11 @@
       <c r="C10" s="8">
         <v>4000</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="8">
         <v>1000</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1856,11 +1919,11 @@
       <c r="B11" s="3">
         <v>3120</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3">
         <v>4000</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1870,11 +1933,25 @@
       <c r="B12" s="3">
         <v>5200</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3">
         <v>9000</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>10</v>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="12">
+        <v>44174</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8000</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1889,26 +1966,26 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="17" style="3" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.8571428571429" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.14285714285714" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.14285714285714" style="3"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1933,11 +2010,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:4">
+    <row r="3" s="2" customFormat="1" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1948,11 +2025,11 @@
       <c r="B4" s="1">
         <v>2080</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>2000</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
@@ -1962,11 +2039,11 @@
       <c r="C5" s="1">
         <v>2000</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1976,11 +2053,25 @@
       <c r="B6" s="3">
         <v>2080</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
         <v>2000</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6">
+        <v>44174</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1996,28 +2087,29 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D1" sqref="D$1:D$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="16.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
+    <col min="1" max="1" width="17" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.8571428571429" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="9.14285714285714" style="7"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -2039,11 +2131,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:4">
+    <row r="3" s="2" customFormat="1" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2054,12 +2146,43 @@
       <c r="B4" s="1">
         <v>1040</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
         <v>1000</v>
       </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6">
+        <v>44174</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6">
+        <v>44174</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2080</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="E6" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2076,8 +2199,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D$1:D$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -2085,15 +2208,15 @@
     <col min="1" max="1" width="17" style="3" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.8571428571429" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.14285714285714" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.14285714285714" style="3"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2118,11 +2241,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:4">
+    <row r="3" s="2" customFormat="1" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2133,11 +2256,11 @@
       <c r="B4" s="1">
         <v>2080</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>2000</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2147,11 +2270,11 @@
       <c r="C5" s="3">
         <v>2000</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3">
         <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2162,4 +2285,20 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>